<commit_message>
Fix Excel export to exactly match template cell positions
</commit_message>
<xml_diff>
--- a/server/templates/export_template.xlsx
+++ b/server/templates/export_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rifqi\OneDrive\Documents\Github\pasir-febrio\server\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rifqi\Downloads\pasir-febrio\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B29B98E-5E2D-46AD-B760-F8EF49541101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F7DC32-4D3F-461D-8B29-8D392E1A535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -186,16 +186,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1. Hutang alat berat 3 unit (HM)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
@@ -207,26 +197,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>2. Hutang Mesin 1 set (HM)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>3. Hutang Royalti (Pak Rizal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
@@ -280,16 +250,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1. Dana Deposit Royalti dari HM…?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
@@ -301,26 +261,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>2. Dana dari Pak Rizal ke HM…?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>3. Dana Pembayaran Tanah …?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
@@ -332,46 +272,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>4. Pengeluaran CBB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>5. Gaji Security CBB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>6. Dana transfer ke HM …?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>7. Discounto ke Pak Alif….?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10.5"/>
         <rFont val="Calibri"/>
@@ -389,46 +289,6 @@
         <family val="1"/>
       </rPr>
       <t>Catatan Beban HO 3:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1. 3 galon meditran</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Rp            1,140,000</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>2. 1 galon meditran</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Rp               528,000</t>
     </r>
   </si>
 </sst>
@@ -436,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -453,13 +313,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -657,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -743,9 +596,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -763,89 +613,86 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1170,66 +1017,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57" t="s">
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1239,9 +1086,9 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="62"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1396,306 +1243,259 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="14" t="s">
         <v>13</v>
       </c>
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="17"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="7"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="55"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="A23" s="50"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="41" t="s">
+      <c r="D23" s="53"/>
+      <c r="E23" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="42"/>
+      <c r="F23" s="57"/>
       <c r="G23" s="20"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A24" s="50"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="19"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="41" t="s">
+      <c r="D24" s="53"/>
+      <c r="E24" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="42"/>
+      <c r="F24" s="57"/>
       <c r="G24" s="10"/>
       <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="42"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="57"/>
       <c r="G25" s="10"/>
       <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="42"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="57"/>
       <c r="G26" s="10"/>
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" s="23"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="45"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="55"/>
       <c r="G27" s="10"/>
       <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="25" t="s">
-        <v>25</v>
-      </c>
+      <c r="A28" s="50"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="45"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="55"/>
       <c r="G28" s="10"/>
       <c r="H28" s="24"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="25" t="s">
-        <v>27</v>
-      </c>
+      <c r="A29" s="50"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="23"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="25" t="s">
-        <v>28</v>
-      </c>
+      <c r="A30" s="50"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="26"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="45"/>
+      <c r="E30" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="55"/>
       <c r="G30" s="10"/>
       <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="25" t="s">
-        <v>32</v>
-      </c>
+      <c r="A33" s="50"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="26"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="25" t="s">
-        <v>33</v>
-      </c>
+      <c r="A34" s="50"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="26"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
+        <v>24</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="31"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
-      <c r="B38" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
-      <c r="B40" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="35">
-        <v>1668000</v>
-      </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="33"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A18:F20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="D37:H40"/>
@@ -1708,6 +1508,23 @@
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="D31:H35"/>
+    <mergeCell ref="A18:F20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add proof image upload for expense transactions
</commit_message>
<xml_diff>
--- a/server/templates/export_template.xlsx
+++ b/server/templates/export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rifqi\Downloads\pasir-febrio\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F7DC32-4D3F-461D-8B29-8D392E1A535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A74C285-6BF9-49D5-BD10-B48017E524A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9D08E"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -510,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -535,12 +536,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -595,9 +590,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -613,6 +605,48 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -652,47 +686,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,7 +1005,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E25" sqref="E25:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1017,66 +1021,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="41" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="56" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1086,9 +1090,9 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="42"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="46"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="57"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1106,47 +1110,47 @@
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="59"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -1155,11 +1159,11 @@
         <v>6</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1167,11 +1171,11 @@
         <v>7</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1179,11 +1183,11 @@
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,11 +1195,11 @@
         <v>9</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1203,299 +1207,316 @@
         <v>10</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="12" t="s">
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="14" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="16" t="s">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="7"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="55"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="56" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="10"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="56" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="20"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="18" t="s">
+      <c r="A25" s="32"/>
+      <c r="B25" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="56" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="20"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="56" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="57"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="20"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="54" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="55"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="24"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="54" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="55"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="24"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="54" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="55"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="24"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="30" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
-      <c r="B40" s="30" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A18:F20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="D37:H40"/>
@@ -1508,23 +1529,6 @@
     <mergeCell ref="D29:H29"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="D31:H35"/>
-    <mergeCell ref="A18:F20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>